<commit_message>
H21 Importacion de modalidad opcion multiple, totalmente funcional
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
+++ b/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ABAABC1-2318-4B47-9A07-F09CD816AF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A6514D-A417-4518-9086-ABE3CE01F155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="oCaxpg8emSD4x0D04aOnZFhmnLUe0JqZ0OE7+OW66+fUILXcAHP8fRQxsDPo8I5QwvOds/Tqxp7HQbl4Th9CLw==" workbookSaltValue="0Z8YzGX+sN4AKivbK0ucJQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
+    <workbookView xWindow="-20610" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Preguntas  de Emparejamiento" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,9 +31,184 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>OpcionCorrecta</t>
+  </si>
+  <si>
+    <t>Opcion</t>
+  </si>
+  <si>
+    <t>Verificacion de plantilla</t>
+  </si>
+  <si>
+    <t>Pregunta 01</t>
+  </si>
+  <si>
+    <t>Pregunta 02</t>
+  </si>
+  <si>
+    <t>Pregunta 03</t>
+  </si>
+  <si>
+    <t>Pregunta 04</t>
+  </si>
+  <si>
+    <t>Pregunta 05</t>
+  </si>
+  <si>
+    <t>Pregunta 06</t>
+  </si>
+  <si>
+    <t>Pregunta 07</t>
+  </si>
+  <si>
+    <t>Pregunta 08</t>
+  </si>
+  <si>
+    <t>Pregunta 09</t>
+  </si>
+  <si>
+    <t>Pregunta 10</t>
+  </si>
+  <si>
+    <t>Pregunta 11</t>
+  </si>
+  <si>
+    <t>Correct 01</t>
+  </si>
+  <si>
+    <t>Correct 02</t>
+  </si>
+  <si>
+    <t>Correct 03</t>
+  </si>
+  <si>
+    <t>Correct 04</t>
+  </si>
+  <si>
+    <t>Correct 05</t>
+  </si>
+  <si>
+    <t>Correct 06</t>
+  </si>
+  <si>
+    <t>Correct 07</t>
+  </si>
+  <si>
+    <t>Correct 08</t>
+  </si>
+  <si>
+    <t>Correct 09</t>
+  </si>
+  <si>
+    <t>Correct 10</t>
+  </si>
+  <si>
+    <t>Correct 11</t>
+  </si>
+  <si>
+    <t>Other 1</t>
+  </si>
+  <si>
+    <t>Other 2</t>
+  </si>
+  <si>
+    <t>Other 3</t>
+  </si>
+  <si>
+    <t>Other 4</t>
+  </si>
+  <si>
+    <t>Other 5</t>
+  </si>
+  <si>
+    <t>Other 6</t>
+  </si>
+  <si>
+    <t>Other 7</t>
+  </si>
+  <si>
+    <t>Other 8</t>
+  </si>
+  <si>
+    <t>Other 9</t>
+  </si>
+  <si>
+    <t>Other 10</t>
+  </si>
+  <si>
+    <t>Other 11</t>
+  </si>
+  <si>
+    <t>Other 1.1</t>
+  </si>
+  <si>
+    <t>Other 1.2</t>
+  </si>
+  <si>
+    <t>Other 1.3</t>
+  </si>
+  <si>
+    <t>Other 1.4</t>
+  </si>
+  <si>
+    <t>Other 1.5</t>
+  </si>
+  <si>
+    <t>Other 1.6</t>
+  </si>
+  <si>
+    <t>Other 1.7</t>
+  </si>
+  <si>
+    <t>Other 1.8</t>
+  </si>
+  <si>
+    <t>Other 1.9</t>
+  </si>
+  <si>
+    <t>Other 1.10</t>
+  </si>
+  <si>
+    <t>Other 1.11</t>
+  </si>
+  <si>
+    <t>1OP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTA: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Es impartente que cada pregunta debe de tener al menos 3 opciones (llenar obligatoriament las columnas B,C y D) si no las posee la pregunta no sera almacenada. Si deja vacia la pregunta no se agregara nada.</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +216,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -57,12 +278,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +754,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82EE6D5-39B6-4ADD-B763-DD534A75A850}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="47.28515625" style="3" customWidth="1"/>
+    <col min="2" max="6" width="15.28515625" style="4"/>
+    <col min="7" max="7" width="15.28515625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="15.28515625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="11"/>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="hvCzrtXIXbP3CYeA4fc4jdnRKEdl4xOrFGoafX2o4dTHV80TjghuBbnypz6ov91CNiKn2pVxk/cEMtVGta+n5w==" saltValue="EpPHe1PcdrPb2fu3yRq9rQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Soporte para multiples opciones en grupo emparejamiento por medio de importacion Excel
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
+++ b/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A6514D-A417-4518-9086-ABE3CE01F155}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="oCaxpg8emSD4x0D04aOnZFhmnLUe0JqZ0OE7+OW66+fUILXcAHP8fRQxsDPo8I5QwvOds/Tqxp7HQbl4Th9CLw==" workbookSaltValue="0Z8YzGX+sN4AKivbK0ucJQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8A8C38-5BBA-4CB2-8403-48F2ED95B2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wGbIgCMq0uujwjh7dBJXO/PI4o/YAxFpGszIEYHZjyYrz6LW89k0jGpVs7ILgjq/YE7LO4DOdCvP/zHPnGE8Uw==" workbookSaltValue="MUMuPjWNCfR+DGRWxpe7pQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
   </bookViews>
   <sheets>
-    <sheet name="Preguntas  de Emparejamiento" sheetId="1" r:id="rId1"/>
+    <sheet name="Preguntas de Opcion Multiple" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -415,29 +415,29 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -757,7 +757,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,27 +769,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="11"/>
-      <c r="G1" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificacion de texto en plantillas excel
</commit_message>
<xml_diff>
--- a/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
+++ b/storage/app/plantillaExcel/ImportarPreguntasOpcionMultiple.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\CICLO VIII\Sistemas 2019\SIGEN_Resources\SIGEN\storage\app\plantillaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8A8C38-5BBA-4CB2-8403-48F2ED95B2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="wGbIgCMq0uujwjh7dBJXO/PI4o/YAxFpGszIEYHZjyYrz6LW89k0jGpVs7ILgjq/YE7LO4DOdCvP/zHPnGE8Uw==" workbookSaltValue="MUMuPjWNCfR+DGRWxpe7pQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB64640-172A-4C92-96D0-2DD1CDB36086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
+    <workbookView xWindow="-20610" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{0622C781-A97F-45D9-9ACD-0F1875EEC481}"/>
   </bookViews>
   <sheets>
     <sheet name="Preguntas de Opcion Multiple" sheetId="1" r:id="rId1"/>
@@ -200,7 +199,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Es impartente que cada pregunta debe de tener al menos 3 opciones (llenar obligatoriament las columnas B,C y D) si no las posee la pregunta no sera almacenada. Si deja vacia la pregunta no se agregara nada.</t>
+      <t>Es importante que cada pregunta debe de tener al menos 3 opciones (llenar obligatoriamente las columnas B,C y D) si no las posee la pregunta no sera almacenada. Si deja vacia la pregunta no se agregara nada.</t>
     </r>
   </si>
 </sst>
@@ -757,7 +756,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +960,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hvCzrtXIXbP3CYeA4fc4jdnRKEdl4xOrFGoafX2o4dTHV80TjghuBbnypz6ov91CNiKn2pVxk/cEMtVGta+n5w==" saltValue="EpPHe1PcdrPb2fu3yRq9rQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Rf7ZGlhBvHsLxsyx4wtjIhIHDpA+bXQ7tPfwE2QbEUhTjTbEyHWsbo7LN37KdhCU4U/aFpaju2oMzVCWASmOGw==" saltValue="cVBovwUAsVOZialvYyyhRg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>